<commit_message>
Update LDLC prices history
</commit_message>
<xml_diff>
--- a/ldlc_suivi_smartphones.xlsx
+++ b/ldlc_suivi_smartphones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>2026-01-27 17:20:17</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2026-01-27 18:21:51</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +479,9 @@
       <c r="D2" t="n">
         <v>45.92</v>
       </c>
+      <c r="E2" t="n">
+        <v>45.92</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +502,9 @@
       <c r="D3" t="n">
         <v>169.95</v>
       </c>
+      <c r="E3" t="n">
+        <v>169.95</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +525,9 @@
       <c r="D4" t="n">
         <v>169.95</v>
       </c>
+      <c r="E4" t="n">
+        <v>169.95</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,6 +548,9 @@
       <c r="D5" t="n">
         <v>179.95</v>
       </c>
+      <c r="E5" t="n">
+        <v>179.95</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +571,9 @@
       <c r="D6" t="n">
         <v>179.95</v>
       </c>
+      <c r="E6" t="n">
+        <v>179.95</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -574,6 +594,9 @@
       <c r="D7" t="n">
         <v>179.95</v>
       </c>
+      <c r="E7" t="n">
+        <v>179.95</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -594,6 +617,9 @@
       <c r="D8" t="n">
         <v>179.95</v>
       </c>
+      <c r="E8" t="n">
+        <v>179.95</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -614,6 +640,9 @@
       <c r="D9" t="n">
         <v>199.95</v>
       </c>
+      <c r="E9" t="n">
+        <v>199.95</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -634,6 +663,9 @@
       <c r="D10" t="n">
         <v>199.95</v>
       </c>
+      <c r="E10" t="n">
+        <v>199.95</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -654,6 +686,9 @@
       <c r="D11" t="n">
         <v>219.95</v>
       </c>
+      <c r="E11" t="n">
+        <v>219.95</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -674,6 +709,9 @@
       <c r="D12" t="n">
         <v>318.95</v>
       </c>
+      <c r="E12" t="n">
+        <v>318.95</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -694,6 +732,9 @@
       <c r="D13" t="n">
         <v>318.95</v>
       </c>
+      <c r="E13" t="n">
+        <v>318.95</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -714,6 +755,9 @@
       <c r="D14" t="n">
         <v>319.95</v>
       </c>
+      <c r="E14" t="n">
+        <v>319.95</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -734,6 +778,9 @@
       <c r="D15" t="n">
         <v>319.95</v>
       </c>
+      <c r="E15" t="n">
+        <v>319.95</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -754,6 +801,9 @@
       <c r="D16" t="n">
         <v>319.95</v>
       </c>
+      <c r="E16" t="n">
+        <v>319.95</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -774,6 +824,9 @@
       <c r="D17" t="n">
         <v>329.95</v>
       </c>
+      <c r="E17" t="n">
+        <v>329.95</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -794,6 +847,9 @@
       <c r="D18" t="n">
         <v>339.95</v>
       </c>
+      <c r="E18" t="n">
+        <v>339.95</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -814,6 +870,9 @@
       <c r="D19" t="n">
         <v>429.95</v>
       </c>
+      <c r="E19" t="n">
+        <v>429.95</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -834,6 +893,9 @@
       <c r="D20" t="n">
         <v>499.95</v>
       </c>
+      <c r="E20" t="n">
+        <v>499.95</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -854,6 +916,9 @@
       <c r="D21" t="n">
         <v>499.95</v>
       </c>
+      <c r="E21" t="n">
+        <v>499.95</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -874,6 +939,9 @@
       <c r="D22" t="n">
         <v>499.95</v>
       </c>
+      <c r="E22" t="n">
+        <v>499.95</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -894,6 +962,9 @@
       <c r="D23" t="n">
         <v>499.95</v>
       </c>
+      <c r="E23" t="n">
+        <v>499.95</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -914,6 +985,9 @@
       <c r="D24" t="n">
         <v>619</v>
       </c>
+      <c r="E24" t="n">
+        <v>619</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -934,6 +1008,9 @@
       <c r="D25" t="n">
         <v>659</v>
       </c>
+      <c r="E25" t="n">
+        <v>659</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -954,6 +1031,9 @@
       <c r="D26" t="n">
         <v>659</v>
       </c>
+      <c r="E26" t="n">
+        <v>659</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -974,6 +1054,9 @@
       <c r="D27" t="n">
         <v>699.95</v>
       </c>
+      <c r="E27" t="n">
+        <v>699.95</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -994,6 +1077,9 @@
       <c r="D28" t="n">
         <v>699.95</v>
       </c>
+      <c r="E28" t="n">
+        <v>699.95</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1014,6 +1100,9 @@
       <c r="D29" t="n">
         <v>699.95</v>
       </c>
+      <c r="E29" t="n">
+        <v>699.95</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1034,6 +1123,9 @@
       <c r="D30" t="n">
         <v>749</v>
       </c>
+      <c r="E30" t="n">
+        <v>749</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1054,6 +1146,9 @@
       <c r="D31" t="n">
         <v>749</v>
       </c>
+      <c r="E31" t="n">
+        <v>749</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1074,6 +1169,9 @@
       <c r="D32" t="n">
         <v>749.95</v>
       </c>
+      <c r="E32" t="n">
+        <v>749.95</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1094,6 +1192,9 @@
       <c r="D33" t="n">
         <v>809</v>
       </c>
+      <c r="E33" t="n">
+        <v>809</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1114,6 +1215,9 @@
       <c r="D34" t="n">
         <v>809</v>
       </c>
+      <c r="E34" t="n">
+        <v>809</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1134,6 +1238,9 @@
       <c r="D35" t="n">
         <v>809</v>
       </c>
+      <c r="E35" t="n">
+        <v>809</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1154,6 +1261,9 @@
       <c r="D36" t="n">
         <v>809</v>
       </c>
+      <c r="E36" t="n">
+        <v>809</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1174,6 +1284,9 @@
       <c r="D37" t="n">
         <v>809</v>
       </c>
+      <c r="E37" t="n">
+        <v>809</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1194,6 +1307,9 @@
       <c r="D38" t="n">
         <v>809.95</v>
       </c>
+      <c r="E38" t="n">
+        <v>809.95</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1214,6 +1330,9 @@
       <c r="D39" t="n">
         <v>849</v>
       </c>
+      <c r="E39" t="n">
+        <v>849</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1234,6 +1353,9 @@
       <c r="D40" t="n">
         <v>899</v>
       </c>
+      <c r="E40" t="n">
+        <v>899</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1254,6 +1376,9 @@
       <c r="D41" t="n">
         <v>899</v>
       </c>
+      <c r="E41" t="n">
+        <v>899</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1274,6 +1399,9 @@
       <c r="D42" t="n">
         <v>909</v>
       </c>
+      <c r="E42" t="n">
+        <v>909</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1294,6 +1422,9 @@
       <c r="D43" t="n">
         <v>909</v>
       </c>
+      <c r="E43" t="n">
+        <v>909</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1314,6 +1445,9 @@
       <c r="D44" t="n">
         <v>909</v>
       </c>
+      <c r="E44" t="n">
+        <v>909</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1334,6 +1468,9 @@
       <c r="D45" t="n">
         <v>969</v>
       </c>
+      <c r="E45" t="n">
+        <v>969</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1354,6 +1491,9 @@
       <c r="D46" t="n">
         <v>969</v>
       </c>
+      <c r="E46" t="n">
+        <v>969</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1374,6 +1514,9 @@
       <c r="D47" t="n">
         <v>969</v>
       </c>
+      <c r="E47" t="n">
+        <v>969</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1394,6 +1537,9 @@
       <c r="D48" t="n">
         <v>969</v>
       </c>
+      <c r="E48" t="n">
+        <v>969</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1414,6 +1560,9 @@
       <c r="D49" t="n">
         <v>969</v>
       </c>
+      <c r="E49" t="n">
+        <v>969</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1434,6 +1583,9 @@
       <c r="D50" t="n">
         <v>999</v>
       </c>
+      <c r="E50" t="n">
+        <v>999</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1454,6 +1606,9 @@
       <c r="D51" t="n">
         <v>999</v>
       </c>
+      <c r="E51" t="n">
+        <v>999</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1474,6 +1629,9 @@
       <c r="D52" t="n">
         <v>1039</v>
       </c>
+      <c r="E52" t="n">
+        <v>1039</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1494,6 +1652,9 @@
       <c r="D53" t="n">
         <v>1039</v>
       </c>
+      <c r="E53" t="n">
+        <v>1039</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1514,6 +1675,9 @@
       <c r="D54" t="n">
         <v>1079</v>
       </c>
+      <c r="E54" t="n">
+        <v>1079</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1534,6 +1698,9 @@
       <c r="D55" t="n">
         <v>1079</v>
       </c>
+      <c r="E55" t="n">
+        <v>1079</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1554,6 +1721,9 @@
       <c r="D56" t="n">
         <v>1079</v>
       </c>
+      <c r="E56" t="n">
+        <v>1079</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1574,6 +1744,9 @@
       <c r="D57" t="n">
         <v>1079</v>
       </c>
+      <c r="E57" t="n">
+        <v>1079</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1594,6 +1767,9 @@
       <c r="D58" t="n">
         <v>1099</v>
       </c>
+      <c r="E58" t="n">
+        <v>1099</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1614,6 +1790,9 @@
       <c r="D59" t="n">
         <v>1099</v>
       </c>
+      <c r="E59" t="n">
+        <v>1099</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1634,6 +1813,9 @@
       <c r="D60" t="n">
         <v>1099</v>
       </c>
+      <c r="E60" t="n">
+        <v>1099</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1654,6 +1836,9 @@
       <c r="D61" t="n">
         <v>1199</v>
       </c>
+      <c r="E61" t="n">
+        <v>1199</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1674,6 +1859,9 @@
       <c r="D62" t="n">
         <v>1219</v>
       </c>
+      <c r="E62" t="n">
+        <v>1219</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1694,6 +1882,9 @@
       <c r="D63" t="n">
         <v>1219</v>
       </c>
+      <c r="E63" t="n">
+        <v>1219</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1714,6 +1905,9 @@
       <c r="D64" t="n">
         <v>1219</v>
       </c>
+      <c r="E64" t="n">
+        <v>1219</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1734,6 +1928,9 @@
       <c r="D65" t="n">
         <v>1219</v>
       </c>
+      <c r="E65" t="n">
+        <v>1219</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1754,6 +1951,9 @@
       <c r="D66" t="n">
         <v>1219</v>
       </c>
+      <c r="E66" t="n">
+        <v>1219</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1774,6 +1974,9 @@
       <c r="D67" t="n">
         <v>1229</v>
       </c>
+      <c r="E67" t="n">
+        <v>1229</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1794,6 +1997,9 @@
       <c r="D68" t="n">
         <v>1229</v>
       </c>
+      <c r="E68" t="n">
+        <v>1229</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1814,6 +2020,9 @@
       <c r="D69" t="n">
         <v>1249</v>
       </c>
+      <c r="E69" t="n">
+        <v>1249</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1834,6 +2043,9 @@
       <c r="D70" t="n">
         <v>1249</v>
       </c>
+      <c r="E70" t="n">
+        <v>1249</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1854,6 +2066,9 @@
       <c r="D71" t="n">
         <v>1329</v>
       </c>
+      <c r="E71" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1874,6 +2089,9 @@
       <c r="D72" t="n">
         <v>1329</v>
       </c>
+      <c r="E72" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1894,6 +2112,9 @@
       <c r="D73" t="n">
         <v>1329</v>
       </c>
+      <c r="E73" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1914,6 +2135,9 @@
       <c r="D74" t="n">
         <v>1329</v>
       </c>
+      <c r="E74" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1934,6 +2158,9 @@
       <c r="D75" t="n">
         <v>1329</v>
       </c>
+      <c r="E75" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1954,6 +2181,9 @@
       <c r="D76" t="n">
         <v>1329</v>
       </c>
+      <c r="E76" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1974,6 +2204,9 @@
       <c r="D77" t="n">
         <v>1329</v>
       </c>
+      <c r="E77" t="n">
+        <v>1329</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1994,6 +2227,9 @@
       <c r="D78" t="n">
         <v>1349</v>
       </c>
+      <c r="E78" t="n">
+        <v>1349</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2014,6 +2250,9 @@
       <c r="D79" t="n">
         <v>1479</v>
       </c>
+      <c r="E79" t="n">
+        <v>1479</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2034,6 +2273,9 @@
       <c r="D80" t="n">
         <v>1479</v>
       </c>
+      <c r="E80" t="n">
+        <v>1479</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2054,6 +2296,9 @@
       <c r="D81" t="n">
         <v>1479</v>
       </c>
+      <c r="E81" t="n">
+        <v>1479</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2074,6 +2319,9 @@
       <c r="D82" t="n">
         <v>1579</v>
       </c>
+      <c r="E82" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2094,6 +2342,9 @@
       <c r="D83" t="n">
         <v>1579</v>
       </c>
+      <c r="E83" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2114,6 +2365,9 @@
       <c r="D84" t="n">
         <v>1579</v>
       </c>
+      <c r="E84" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2134,6 +2388,9 @@
       <c r="D85" t="n">
         <v>1579</v>
       </c>
+      <c r="E85" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2154,6 +2411,9 @@
       <c r="D86" t="n">
         <v>1579</v>
       </c>
+      <c r="E86" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2174,6 +2434,9 @@
       <c r="D87" t="n">
         <v>1579</v>
       </c>
+      <c r="E87" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2194,6 +2457,9 @@
       <c r="D88" t="n">
         <v>1579</v>
       </c>
+      <c r="E88" t="n">
+        <v>1579</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2214,6 +2480,9 @@
       <c r="D89" t="n">
         <v>1729</v>
       </c>
+      <c r="E89" t="n">
+        <v>1729</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2234,6 +2503,9 @@
       <c r="D90" t="n">
         <v>1729</v>
       </c>
+      <c r="E90" t="n">
+        <v>1729</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2254,6 +2526,9 @@
       <c r="D91" t="n">
         <v>1729</v>
       </c>
+      <c r="E91" t="n">
+        <v>1729</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2274,6 +2549,9 @@
       <c r="D92" t="n">
         <v>1829</v>
       </c>
+      <c r="E92" t="n">
+        <v>1829</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2294,6 +2572,9 @@
       <c r="D93" t="n">
         <v>1829</v>
       </c>
+      <c r="E93" t="n">
+        <v>1829</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2314,6 +2595,9 @@
       <c r="D94" t="n">
         <v>1829</v>
       </c>
+      <c r="E94" t="n">
+        <v>1829</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2334,6 +2618,9 @@
       <c r="D95" t="n">
         <v>1979</v>
       </c>
+      <c r="E95" t="n">
+        <v>1979</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2354,6 +2641,9 @@
       <c r="D96" t="n">
         <v>1979</v>
       </c>
+      <c r="E96" t="n">
+        <v>1979</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2374,6 +2664,9 @@
       <c r="D97" t="n">
         <v>1979</v>
       </c>
+      <c r="E97" t="n">
+        <v>1979</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2394,6 +2687,9 @@
       <c r="D98" t="n">
         <v>2479</v>
       </c>
+      <c r="E98" t="n">
+        <v>2479</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2414,6 +2710,9 @@
       <c r="D99" t="n">
         <v>2479</v>
       </c>
+      <c r="E99" t="n">
+        <v>2479</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2434,6 +2733,9 @@
       <c r="D100" t="n">
         <v>2479</v>
       </c>
+      <c r="E100" t="n">
+        <v>2479</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2452,6 +2754,7 @@
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2470,6 +2773,7 @@
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2488,6 +2792,7 @@
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2506,6 +2811,7 @@
         </is>
       </c>
       <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2524,6 +2830,7 @@
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2542,6 +2849,7 @@
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2560,6 +2868,7 @@
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2578,6 +2887,7 @@
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2596,6 +2906,7 @@
         </is>
       </c>
       <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2614,6 +2925,7 @@
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2632,6 +2944,7 @@
         </is>
       </c>
       <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2650,6 +2963,7 @@
         </is>
       </c>
       <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2668,6 +2982,7 @@
         </is>
       </c>
       <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2686,6 +3001,7 @@
         </is>
       </c>
       <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2704,6 +3020,7 @@
         </is>
       </c>
       <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2722,6 +3039,7 @@
         </is>
       </c>
       <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2740,6 +3058,7 @@
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2758,6 +3077,7 @@
         </is>
       </c>
       <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2776,6 +3096,7 @@
         </is>
       </c>
       <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2794,6 +3115,7 @@
         </is>
       </c>
       <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2812,6 +3134,7 @@
         </is>
       </c>
       <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2830,6 +3153,7 @@
         </is>
       </c>
       <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2848,6 +3172,7 @@
         </is>
       </c>
       <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2866,6 +3191,7 @@
         </is>
       </c>
       <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2884,6 +3210,7 @@
         </is>
       </c>
       <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2902,6 +3229,7 @@
         </is>
       </c>
       <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2920,6 +3248,7 @@
         </is>
       </c>
       <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2938,6 +3267,7 @@
         </is>
       </c>
       <c r="D128" t="inlineStr"/>
+      <c r="E128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2956,6 +3286,7 @@
         </is>
       </c>
       <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2974,6 +3305,7 @@
         </is>
       </c>
       <c r="D130" t="inlineStr"/>
+      <c r="E130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2992,6 +3324,7 @@
         </is>
       </c>
       <c r="D131" t="inlineStr"/>
+      <c r="E131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3010,6 +3343,7 @@
         </is>
       </c>
       <c r="D132" t="inlineStr"/>
+      <c r="E132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3028,6 +3362,7 @@
         </is>
       </c>
       <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3046,6 +3381,7 @@
         </is>
       </c>
       <c r="D134" t="inlineStr"/>
+      <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3064,6 +3400,7 @@
         </is>
       </c>
       <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3082,6 +3419,7 @@
         </is>
       </c>
       <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3100,6 +3438,7 @@
         </is>
       </c>
       <c r="D137" t="inlineStr"/>
+      <c r="E137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3118,6 +3457,7 @@
         </is>
       </c>
       <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3136,6 +3476,7 @@
         </is>
       </c>
       <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3154,6 +3495,7 @@
         </is>
       </c>
       <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3172,6 +3514,7 @@
         </is>
       </c>
       <c r="D141" t="inlineStr"/>
+      <c r="E141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3190,6 +3533,7 @@
         </is>
       </c>
       <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3208,6 +3552,7 @@
         </is>
       </c>
       <c r="D143" t="inlineStr"/>
+      <c r="E143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3226,6 +3571,7 @@
         </is>
       </c>
       <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3244,6 +3590,7 @@
         </is>
       </c>
       <c r="D145" t="inlineStr"/>
+      <c r="E145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3262,6 +3609,7 @@
         </is>
       </c>
       <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3280,6 +3628,7 @@
         </is>
       </c>
       <c r="D147" t="inlineStr"/>
+      <c r="E147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -3298,6 +3647,7 @@
         </is>
       </c>
       <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3316,6 +3666,7 @@
         </is>
       </c>
       <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -3334,6 +3685,7 @@
         </is>
       </c>
       <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -3352,6 +3704,7 @@
         </is>
       </c>
       <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3370,6 +3723,7 @@
         </is>
       </c>
       <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3388,6 +3742,7 @@
         </is>
       </c>
       <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3406,6 +3761,7 @@
         </is>
       </c>
       <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3424,6 +3780,7 @@
         </is>
       </c>
       <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3442,6 +3799,7 @@
         </is>
       </c>
       <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3460,6 +3818,7 @@
         </is>
       </c>
       <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3478,6 +3837,7 @@
         </is>
       </c>
       <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3496,6 +3856,7 @@
         </is>
       </c>
       <c r="D159" t="inlineStr"/>
+      <c r="E159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3514,6 +3875,7 @@
         </is>
       </c>
       <c r="D160" t="inlineStr"/>
+      <c r="E160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3532,6 +3894,7 @@
         </is>
       </c>
       <c r="D161" t="inlineStr"/>
+      <c r="E161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -3550,6 +3913,7 @@
         </is>
       </c>
       <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -3568,6 +3932,7 @@
         </is>
       </c>
       <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -3586,6 +3951,7 @@
         </is>
       </c>
       <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -3604,6 +3970,7 @@
         </is>
       </c>
       <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -3622,6 +3989,7 @@
         </is>
       </c>
       <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -3640,6 +4008,7 @@
         </is>
       </c>
       <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -3658,6 +4027,7 @@
         </is>
       </c>
       <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3676,6 +4046,7 @@
         </is>
       </c>
       <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -3694,6 +4065,7 @@
         </is>
       </c>
       <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3712,6 +4084,7 @@
         </is>
       </c>
       <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -3730,6 +4103,7 @@
         </is>
       </c>
       <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -3748,6 +4122,7 @@
         </is>
       </c>
       <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3766,6 +4141,7 @@
         </is>
       </c>
       <c r="D174" t="inlineStr"/>
+      <c r="E174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3784,6 +4160,7 @@
         </is>
       </c>
       <c r="D175" t="inlineStr"/>
+      <c r="E175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3802,6 +4179,7 @@
         </is>
       </c>
       <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3820,6 +4198,7 @@
         </is>
       </c>
       <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -3838,6 +4217,7 @@
         </is>
       </c>
       <c r="D178" t="inlineStr"/>
+      <c r="E178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -3856,6 +4236,7 @@
         </is>
       </c>
       <c r="D179" t="inlineStr"/>
+      <c r="E179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -3874,6 +4255,7 @@
         </is>
       </c>
       <c r="D180" t="inlineStr"/>
+      <c r="E180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -3892,6 +4274,7 @@
         </is>
       </c>
       <c r="D181" t="inlineStr"/>
+      <c r="E181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -3910,6 +4293,7 @@
         </is>
       </c>
       <c r="D182" t="inlineStr"/>
+      <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -3928,6 +4312,7 @@
         </is>
       </c>
       <c r="D183" t="inlineStr"/>
+      <c r="E183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -3946,6 +4331,7 @@
         </is>
       </c>
       <c r="D184" t="inlineStr"/>
+      <c r="E184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -3964,6 +4350,7 @@
         </is>
       </c>
       <c r="D185" t="inlineStr"/>
+      <c r="E185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -3982,6 +4369,7 @@
         </is>
       </c>
       <c r="D186" t="inlineStr"/>
+      <c r="E186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4000,6 +4388,7 @@
         </is>
       </c>
       <c r="D187" t="inlineStr"/>
+      <c r="E187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4018,6 +4407,7 @@
         </is>
       </c>
       <c r="D188" t="inlineStr"/>
+      <c r="E188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4036,6 +4426,7 @@
         </is>
       </c>
       <c r="D189" t="inlineStr"/>
+      <c r="E189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4054,6 +4445,7 @@
         </is>
       </c>
       <c r="D190" t="inlineStr"/>
+      <c r="E190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4072,6 +4464,7 @@
         </is>
       </c>
       <c r="D191" t="inlineStr"/>
+      <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4090,6 +4483,7 @@
         </is>
       </c>
       <c r="D192" t="inlineStr"/>
+      <c r="E192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4108,6 +4502,7 @@
         </is>
       </c>
       <c r="D193" t="inlineStr"/>
+      <c r="E193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4126,6 +4521,7 @@
         </is>
       </c>
       <c r="D194" t="inlineStr"/>
+      <c r="E194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4144,6 +4540,7 @@
         </is>
       </c>
       <c r="D195" t="inlineStr"/>
+      <c r="E195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4162,6 +4559,7 @@
         </is>
       </c>
       <c r="D196" t="inlineStr"/>
+      <c r="E196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4180,6 +4578,7 @@
         </is>
       </c>
       <c r="D197" t="inlineStr"/>
+      <c r="E197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -4198,6 +4597,7 @@
         </is>
       </c>
       <c r="D198" t="inlineStr"/>
+      <c r="E198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -4216,6 +4616,7 @@
         </is>
       </c>
       <c r="D199" t="inlineStr"/>
+      <c r="E199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -4234,6 +4635,7 @@
         </is>
       </c>
       <c r="D200" t="inlineStr"/>
+      <c r="E200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -4252,6 +4654,7 @@
         </is>
       </c>
       <c r="D201" t="inlineStr"/>
+      <c r="E201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -4270,6 +4673,7 @@
         </is>
       </c>
       <c r="D202" t="inlineStr"/>
+      <c r="E202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -4288,6 +4692,7 @@
         </is>
       </c>
       <c r="D203" t="inlineStr"/>
+      <c r="E203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -4306,6 +4711,7 @@
         </is>
       </c>
       <c r="D204" t="inlineStr"/>
+      <c r="E204" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>